<commit_message>
Modified more excel sheets.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-1_no-graph.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-1_no-graph.xlsx
@@ -597,7 +597,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A9" sqref="A9:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1919,7 +1919,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>